<commit_message>
actualización diccionario de variables
</commit_message>
<xml_diff>
--- a/Equip_E/Data/dicionario de variables.xlsx
+++ b/Equip_E/Data/dicionario de variables.xlsx
@@ -20,7 +20,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Descripción y características
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Anuncios de inmuebles de alquiler turístico en las principales plataformas.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Las características de este dataset son las siguientes:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Volumen estimado: 25000 registros cada 7 días
+Histórico: disponible desde 2017-01</t>
+    </r>
+  </si>
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -266,7 +315,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -288,6 +337,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -352,16 +416,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,13 +552,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>256320</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>66600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>463320</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:colOff>462960</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -500,8 +572,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="256320" y="7667640"/>
-          <a:ext cx="8921160" cy="1257480"/>
+          <a:off x="256320" y="8681760"/>
+          <a:ext cx="8920800" cy="1257120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -694,520 +766,531 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="81"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="2" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="2" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="2" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="2" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" s="2" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="2" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="2" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="B37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B36">
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B3:B37">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"int64"</formula>
     </cfRule>
@@ -1218,7 +1301,7 @@
       <formula>"object"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C36">
+  <conditionalFormatting sqref="C3:C37">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"categórica"</formula>
     </cfRule>
@@ -1227,7 +1310,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="C2:C36" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="C3:C37" type="list">
       <formula1>"numérica,categórica"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>